<commit_message>
Atualização do banco de dados Regiões
</commit_message>
<xml_diff>
--- a/Curso R/bd/regioes.xlsx
+++ b/Curso R/bd/regioes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="69">
   <si>
     <t>uf</t>
   </si>
@@ -560,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -585,7 +585,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -651,10 +651,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
@@ -662,18 +662,18 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -750,18 +750,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -794,18 +794,18 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -827,18 +827,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -860,12 +860,23 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>5</v>
       </c>
       <c r="C27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>53</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>